<commit_message>
Addig upload field to the RuleItem
</commit_message>
<xml_diff>
--- a/src/main/resources/time_conversion_rules1.xlsx
+++ b/src/main/resources/time_conversion_rules1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="132">
   <si>
     <t xml:space="preserve">colMarkID</t>
   </si>
@@ -49,6 +49,9 @@
     <t xml:space="preserve">Column3</t>
   </si>
   <si>
+    <t xml:space="preserve">Выгружать</t>
+  </si>
+  <si>
     <t xml:space="preserve">рв</t>
   </si>
   <si>
@@ -58,6 +61,9 @@
     <t xml:space="preserve">Години роботи у вихідні й святкові дні</t>
   </si>
   <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
     <t xml:space="preserve">д</t>
   </si>
   <si>
@@ -68,6 +74,9 @@
   </si>
   <si>
     <t xml:space="preserve">Години роботи, передбачені колдоговором</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
   </si>
   <si>
     <t xml:space="preserve">пр</t>
@@ -421,6 +430,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -502,15 +512,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="I34" activeCellId="0" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.24489795918367"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.16836734693878"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="144.081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -541,34 +555,40 @@
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>5</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>9</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>6</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -576,10 +596,10 @@
         <v>21</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>1</v>
@@ -591,13 +611,16 @@
         <v>4</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -605,10 +628,10 @@
         <v>94</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>1</v>
@@ -620,13 +643,16 @@
         <v>1</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -634,10 +660,10 @@
         <v>104</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>1</v>
@@ -649,13 +675,16 @@
         <v>1</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -663,10 +692,10 @@
         <v>107</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>1</v>
@@ -678,13 +707,16 @@
         <v>1</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -692,10 +724,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>0</v>
@@ -707,13 +739,16 @@
         <v>4</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -721,10 +756,10 @@
         <v>2</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>0</v>
@@ -736,13 +771,16 @@
         <v>4</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>4</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -750,10 +788,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>1</v>
@@ -765,13 +803,16 @@
         <v>4</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H9" s="0" t="n">
         <v>7</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -779,10 +820,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>1</v>
@@ -794,13 +835,16 @@
         <v>8</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>27</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -808,10 +852,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>1</v>
@@ -823,13 +867,16 @@
         <v>8</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H11" s="0" t="n">
         <v>18</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -837,10 +884,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>1</v>
@@ -852,13 +899,16 @@
         <v>4</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H12" s="0" t="n">
         <v>8</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -866,10 +916,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>1</v>
@@ -881,13 +931,16 @@
         <v>4</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="H13" s="0" t="n">
         <v>14</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -895,10 +948,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>1</v>
@@ -910,13 +963,16 @@
         <v>4</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="H14" s="0" t="n">
         <v>12</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -924,10 +980,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>1</v>
@@ -939,13 +995,16 @@
         <v>4</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>13</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -953,28 +1012,31 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C16" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G16" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="D16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>46</v>
       </c>
       <c r="H16" s="0" t="n">
         <v>13</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -982,10 +1044,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>1</v>
@@ -997,13 +1059,16 @@
         <v>4</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H17" s="0" t="n">
         <v>6</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1011,10 +1076,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>1</v>
@@ -1026,13 +1091,16 @@
         <v>4</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H18" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1040,10 +1108,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>1</v>
@@ -1055,13 +1123,16 @@
         <v>4</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H19" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1069,10 +1140,10 @@
         <v>22</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>1</v>
@@ -1084,13 +1155,16 @@
         <v>4</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H20" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1098,10 +1172,10 @@
         <v>23</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>0</v>
@@ -1113,13 +1187,16 @@
         <v>4</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H21" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1127,10 +1204,10 @@
         <v>25</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>1</v>
@@ -1142,13 +1219,16 @@
         <v>4</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H22" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1156,10 +1236,10 @@
         <v>26</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>1</v>
@@ -1171,13 +1251,16 @@
         <v>4</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H23" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1185,10 +1268,10 @@
         <v>27</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>1</v>
@@ -1200,13 +1283,16 @@
         <v>4</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H24" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1214,10 +1300,10 @@
         <v>28</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>1</v>
@@ -1229,13 +1315,16 @@
         <v>4</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H25" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1243,10 +1332,10 @@
         <v>29</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>1</v>
@@ -1258,13 +1347,16 @@
         <v>4</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H26" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J26" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1272,10 +1364,10 @@
         <v>30</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>0</v>
@@ -1287,13 +1379,16 @@
         <v>4</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H27" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1301,10 +1396,10 @@
         <v>31</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>1</v>
@@ -1316,13 +1411,16 @@
         <v>4</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H28" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J28" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1330,10 +1428,10 @@
         <v>33</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>1</v>
@@ -1345,13 +1443,16 @@
         <v>4</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H29" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J29" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1359,10 +1460,10 @@
         <v>34</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>1</v>
@@ -1374,13 +1475,16 @@
         <v>4</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H30" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J30" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1388,10 +1492,10 @@
         <v>36</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>1</v>
@@ -1403,13 +1507,16 @@
         <v>4</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H31" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J31" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1417,10 +1524,10 @@
         <v>39</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>0</v>
@@ -1432,13 +1539,16 @@
         <v>1</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H32" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J32" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1446,10 +1556,10 @@
         <v>40</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>1</v>
@@ -1461,13 +1571,16 @@
         <v>4</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H33" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J33" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1475,10 +1588,10 @@
         <v>44</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>0</v>
@@ -1490,13 +1603,16 @@
         <v>1</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H34" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J34" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1504,10 +1620,10 @@
         <v>60</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>0</v>
@@ -1519,13 +1635,16 @@
         <v>1</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H35" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J35" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1533,10 +1652,10 @@
         <v>70</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>0</v>
@@ -1548,13 +1667,16 @@
         <v>1</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H36" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J36" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1562,10 +1684,10 @@
         <v>71</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>0</v>
@@ -1577,13 +1699,16 @@
         <v>1</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H37" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J37" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1591,10 +1716,10 @@
         <v>81</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>0</v>
@@ -1606,13 +1731,16 @@
         <v>1</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H38" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I38" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J38" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1620,10 +1748,10 @@
         <v>90</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>0</v>
@@ -1635,13 +1763,16 @@
         <v>1</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H39" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I39" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J39" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1649,10 +1780,10 @@
         <v>92</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>0</v>
@@ -1664,13 +1795,16 @@
         <v>4</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H40" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I40" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J40" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1678,10 +1812,10 @@
         <v>93</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D41" s="0" t="n">
         <v>1</v>
@@ -1693,13 +1827,16 @@
         <v>1</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H41" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I41" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J41" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1707,10 +1844,10 @@
         <v>96</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D42" s="0" t="n">
         <v>1</v>
@@ -1722,13 +1859,16 @@
         <v>1</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="H42" s="0" t="n">
         <v>26</v>
       </c>
       <c r="I42" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
+      </c>
+      <c r="J42" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1736,10 +1876,10 @@
         <v>97</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D43" s="0" t="n">
         <v>1</v>
@@ -1751,13 +1891,16 @@
         <v>1</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="H43" s="0" t="n">
         <v>16</v>
       </c>
       <c r="I43" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
+      </c>
+      <c r="J43" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1765,10 +1908,10 @@
         <v>98</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D44" s="0" t="n">
         <v>1</v>
@@ -1780,13 +1923,16 @@
         <v>1</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H44" s="0" t="n">
         <v>8</v>
       </c>
       <c r="I44" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="J44" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1794,10 +1940,10 @@
         <v>100</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D45" s="0" t="n">
         <v>1</v>
@@ -1809,13 +1955,16 @@
         <v>1</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="H45" s="0" t="n">
         <v>19</v>
       </c>
       <c r="I45" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
+      </c>
+      <c r="J45" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1823,10 +1972,10 @@
         <v>101</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D46" s="0" t="n">
         <v>1</v>
@@ -1838,13 +1987,16 @@
         <v>1</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H46" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I46" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J46" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1852,10 +2004,10 @@
         <v>102</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D47" s="0" t="n">
         <v>1</v>
@@ -1867,13 +2019,16 @@
         <v>1</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H47" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J47" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1881,10 +2036,10 @@
         <v>103</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D48" s="0" t="n">
         <v>1</v>
@@ -1896,13 +2051,16 @@
         <v>1</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H48" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J48" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1910,10 +2068,10 @@
         <v>105</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D49" s="0" t="n">
         <v>1</v>
@@ -1925,13 +2083,16 @@
         <v>1</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H49" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J49" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1939,10 +2100,10 @@
         <v>108</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D50" s="0" t="n">
         <v>1</v>
@@ -1954,13 +2115,16 @@
         <v>1</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H50" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I50" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J50" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1968,10 +2132,10 @@
         <v>109</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D51" s="0" t="n">
         <v>0</v>
@@ -1983,13 +2147,16 @@
         <v>1</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H51" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I51" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J51" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1997,10 +2164,10 @@
         <v>110</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D52" s="0" t="n">
         <v>0</v>
@@ -2012,13 +2179,16 @@
         <v>1</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H52" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I52" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J52" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2026,10 +2196,10 @@
         <v>116</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D53" s="0" t="n">
         <v>4</v>
@@ -2041,13 +2211,16 @@
         <v>1</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H53" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I53" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J53" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2055,10 +2228,10 @@
         <v>119</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D54" s="0" t="n">
         <v>4</v>
@@ -2070,13 +2243,16 @@
         <v>1</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H54" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I54" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="J54" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>